<commit_message>
fix format curcency and reacycle bin
</commit_message>
<xml_diff>
--- a/Testcase_eazysell.xlsx
+++ b/Testcase_eazysell.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="75">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -233,49 +233,7 @@
     <t>Eazysell</t>
   </si>
   <si>
-    <t>Đăng nhập thành công vào phần mềm</t>
-  </si>
-  <si>
-    <t>Đăng nhập thành công vào phần mềm với tài khoản được chỉ định</t>
-  </si>
-  <si>
-    <t>Đăng nhập thành công vô tài khoản</t>
-  </si>
-  <si>
     <t>1.1.1 Chức năng đăng nhập</t>
-  </si>
-  <si>
-    <t>Đăng nhập với tài khoản sai</t>
-  </si>
-  <si>
-    <t>Không thể đăng nhập với tài khoản sai</t>
-  </si>
-  <si>
-    <t>1.Mở website:http://bachhoa.test:8080/
-2.Nhập tên đăng nhập: admin
-3.Nhập mật khẩu:12345678
-4. Nhấn nút đăng nhập</t>
-  </si>
-  <si>
-    <t>1.Mở website: http://bachhoa.test:8080/
-2.Nhập tên đăng nhập: test
-3.Nhập mật khẩu:12345678
-4. Nhấn nút đăng nhập</t>
-  </si>
-  <si>
-    <t>Không đăng nhập thành công và hiển thị thông báo sai mật khẩu hoặc sai tên đăng nhập</t>
-  </si>
-  <si>
-    <t>Đăng nhập với mật khẩu ít hơn 8 ký tự</t>
-  </si>
-  <si>
-    <t>Đăng nhập vào tài khoản với mật khẩu ít hơn 8 ký tự</t>
-  </si>
-  <si>
-    <t>1.Mở website: http://bachhoa.test:8080/
-2.Nhập tên đăng nhập: test
-3.Nhập mật khẩu:123
-4. Nhấn nút đăng nhập</t>
   </si>
   <si>
     <t>Không đăng nhập thành công và hiển thị thông báo mật khẩu phải có ít nhất 8 ký tự</t>
@@ -291,6 +249,54 @@
 2.Nhấn đăng ký
 3.Nhập mật khẩu:123
 4. Nhấn nút đăng nhập</t>
+  </si>
+  <si>
+    <t>Thông báo đăng ký tài khoản thành công</t>
+  </si>
+  <si>
+    <t>Nhập mật khẩu</t>
+  </si>
+  <si>
+    <t>Login was successful in the software</t>
+  </si>
+  <si>
+    <t>Login was successful in the software with a valid account</t>
+  </si>
+  <si>
+    <t>1.Open website:http://bachhoa.test:8080/
+2.Input username: admin
+3.Input password:12345678
+4. Click on login button</t>
+  </si>
+  <si>
+    <t>Login with wrong account</t>
+  </si>
+  <si>
+    <t>Cannot login with the wrong account</t>
+  </si>
+  <si>
+    <t>1.Open website:http://bachhoa.test:8080/
+2.Input username: abc
+3.Input password:12345678
+4. Click on login button</t>
+  </si>
+  <si>
+    <t>Login successfully</t>
+  </si>
+  <si>
+    <t>Login denied with a notification:"Cannot log in because the username or password incorrect'</t>
+  </si>
+  <si>
+    <t>Login with a password that has a lenghth less than 8 characters</t>
+  </si>
+  <si>
+    <t>Input a password that has a length less than 8 characters</t>
+  </si>
+  <si>
+    <t>1.Open website:http://bachhoa.test:8080/
+2.Input username: admin
+3.Input password:abc12
+4. Click on login button</t>
   </si>
 </sst>
 </file>
@@ -30043,7 +30049,7 @@
       <c r="F5" s="146"/>
       <c r="G5" s="158">
         <f ca="1">NOW()</f>
-        <v>45227.374748263886</v>
+        <v>45233.383203472222</v>
       </c>
       <c r="H5" s="159"/>
       <c r="I5" s="26"/>
@@ -58033,8 +58039,8 @@
   </sheetPr>
   <dimension ref="A1:Z856"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -58372,7 +58378,7 @@
     <row r="10" spans="1:26">
       <c r="A10" s="132"/>
       <c r="B10" s="133" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="134"/>
       <c r="D10" s="133"/>
@@ -58405,16 +58411,16 @@
         <v>[Eazysell-2]</v>
       </c>
       <c r="B11" s="138" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C11" s="138" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D11" s="139" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E11" s="143" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F11" s="140" t="s">
         <v>18</v>
@@ -58449,16 +58455,16 @@
         <v>[Eazysell-2]</v>
       </c>
       <c r="B12" s="138" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C12" s="138" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D12" s="139" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E12" s="143" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F12" s="140" t="s">
         <v>18</v>
@@ -58476,16 +58482,16 @@
         <v>[Eazysell-3]</v>
       </c>
       <c r="B13" s="138" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C13" s="138" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D13" s="139" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E13" s="143" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F13" s="140" t="s">
         <v>18</v>
@@ -58500,7 +58506,7 @@
     <row r="14" spans="1:26">
       <c r="A14" s="132"/>
       <c r="B14" s="133" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C14" s="134"/>
       <c r="D14" s="133"/>
@@ -58530,18 +58536,20 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="142" t="str">
         <f>IF(AND(E15=""),"","["&amp;TEXT($B$1,"##")&amp;"-"&amp;TEXT(ROW()-9- COUNTBLANK($E$8:E13) +1,"##")&amp;"]")</f>
-        <v/>
+        <v>[Eazysell-5]</v>
       </c>
       <c r="B15" s="138" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C15" s="138" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D15" s="139" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="143"/>
+        <v>61</v>
+      </c>
+      <c r="E15" s="143" t="s">
+        <v>62</v>
+      </c>
       <c r="F15" s="140" t="s">
         <v>18</v>
       </c>
@@ -58557,7 +58565,9 @@
         <f>IF(AND(E16=""),"","["&amp;TEXT($B$1,"##")&amp;"-"&amp;TEXT(ROW()-9- COUNTBLANK($E$8:E14) +1,"##")&amp;"]")</f>
         <v/>
       </c>
-      <c r="B16" s="138"/>
+      <c r="B16" s="138" t="s">
+        <v>63</v>
+      </c>
       <c r="C16" s="138"/>
       <c r="D16" s="139"/>
       <c r="E16" s="143"/>

</xml_diff>